<commit_message>
entity_template TR damage function added
template damage function for TR (tropical cyclone rain) added
</commit_message>
<xml_diff>
--- a/data/entities/entity_template.xlsx
+++ b/data/entities/entity_template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="620" windowWidth="24460" windowHeight="12480" tabRatio="766" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14820" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -260,11 +260,12 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>added 20141222</t>
+          <t>added 20141222
+20160529, replaced with a reasonable damage function (inspired byEQ California, expert guess)</t>
         </r>
       </text>
     </comment>
-    <comment ref="A86" authorId="1">
+    <comment ref="A81" authorId="1">
       <text>
         <r>
           <rPr>
@@ -277,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F86" authorId="0">
+    <comment ref="F81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -286,6 +287,31 @@
             <rFont val="Arial"/>
           </rPr>
           <t>climada_damagefunction_generate(0:10:500,0,1,0.75,'s-shape','VQ')</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B132" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>20160529 added to just to have something in. Copy/paste from TC, indensity multiplied by 10 (to cover up to 1200 mm of rain, then last lines 1500, 2000 and 3000 added.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F132" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>climada_damagefunction_generate(0:5:120,25,1,0.375,'s-shape','TC',0);</t>
         </r>
       </text>
     </comment>
@@ -775,7 +801,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="83">
   <si>
     <t>Latitude</t>
   </si>
@@ -1091,17 +1117,20 @@
   <si>
     <t>THIS tab contains OLD damagefunctions (just to keep track, not in use)</t>
   </si>
+  <si>
+    <t>TR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1204,7 +1233,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1253,6 +1282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1289,69 +1324,69 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -1359,23 +1394,23 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="13" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="13" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1385,9 +1420,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="5" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2344,10 +2384,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.33203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3744,15 +3784,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="58">
-        <v>1</v>
-      </c>
-      <c r="B67" s="59">
-        <v>4</v>
-      </c>
-      <c r="C67" s="60">
-        <v>1E-3</v>
+    <row r="67" spans="1:6" s="90" customFormat="1">
+      <c r="A67" s="89">
+        <v>1</v>
+      </c>
+      <c r="B67" s="40">
+        <v>0</v>
+      </c>
+      <c r="C67" s="39">
+        <v>0</v>
       </c>
       <c r="D67" s="61">
         <v>0</v>
@@ -3761,386 +3801,386 @@
         <f>C67*D67</f>
         <v>0</v>
       </c>
-      <c r="F67" s="59" t="s">
+      <c r="F67" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="58">
-        <v>1</v>
-      </c>
-      <c r="B68" s="59">
-        <v>4.5</v>
-      </c>
-      <c r="C68" s="60">
-        <v>0.01</v>
+    <row r="68" spans="1:6" s="90" customFormat="1">
+      <c r="A68" s="89">
+        <v>1</v>
+      </c>
+      <c r="B68" s="40">
+        <v>1</v>
+      </c>
+      <c r="C68" s="39">
+        <v>0</v>
       </c>
       <c r="D68" s="61">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E68" s="61">
-        <f t="shared" ref="E68:E85" si="3">C68*D68</f>
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F68" s="59" t="s">
+        <f t="shared" ref="E68:E80" si="3">C68*D68</f>
+        <v>0</v>
+      </c>
+      <c r="F68" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="58">
-        <v>1</v>
-      </c>
-      <c r="B69" s="59">
-        <v>5</v>
-      </c>
-      <c r="C69" s="60">
-        <v>0.02</v>
+    <row r="69" spans="1:6" s="90" customFormat="1">
+      <c r="A69" s="89">
+        <v>1</v>
+      </c>
+      <c r="B69" s="40">
+        <v>2</v>
+      </c>
+      <c r="C69" s="39">
+        <v>0</v>
       </c>
       <c r="D69" s="61">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E69" s="61">
         <f t="shared" si="3"/>
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="F69" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="F69" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="58">
-        <v>1</v>
-      </c>
-      <c r="B70" s="59">
-        <v>5.5</v>
-      </c>
-      <c r="C70" s="60">
-        <v>2.3E-2</v>
+    <row r="70" spans="1:6" s="90" customFormat="1">
+      <c r="A70" s="89">
+        <v>1</v>
+      </c>
+      <c r="B70" s="40">
+        <v>3</v>
+      </c>
+      <c r="C70" s="39">
+        <v>0</v>
       </c>
       <c r="D70" s="61">
-        <v>4.1000000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="E70" s="61">
         <f t="shared" si="3"/>
-        <v>9.4300000000000004E-4</v>
-      </c>
-      <c r="F70" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="F70" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="58">
-        <v>1</v>
-      </c>
-      <c r="B71" s="59">
-        <v>6</v>
-      </c>
-      <c r="C71" s="60">
-        <v>0.03</v>
+    <row r="71" spans="1:6" s="90" customFormat="1">
+      <c r="A71" s="89">
+        <v>1</v>
+      </c>
+      <c r="B71" s="40">
+        <v>4</v>
+      </c>
+      <c r="C71" s="39">
+        <v>0</v>
       </c>
       <c r="D71" s="61">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E71" s="61">
         <f t="shared" si="3"/>
-        <v>1.5E-3</v>
-      </c>
-      <c r="F71" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="58">
-        <v>1</v>
-      </c>
-      <c r="B72" s="59">
-        <v>6.5</v>
-      </c>
-      <c r="C72" s="60">
-        <v>0.04</v>
+    <row r="72" spans="1:6" s="90" customFormat="1">
+      <c r="A72" s="89">
+        <v>1</v>
+      </c>
+      <c r="B72" s="40">
+        <v>5</v>
+      </c>
+      <c r="C72" s="39">
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="D72" s="61">
-        <v>7.0000000000000007E-2</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="E72" s="61">
         <f t="shared" si="3"/>
-        <v>2.8000000000000004E-3</v>
-      </c>
-      <c r="F72" s="59" t="s">
+        <v>9.0249999999999998E-5</v>
+      </c>
+      <c r="F72" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="58">
-        <v>1</v>
-      </c>
-      <c r="B73" s="59">
-        <v>7</v>
-      </c>
-      <c r="C73" s="60">
-        <v>0.06</v>
+    <row r="73" spans="1:6" s="90" customFormat="1">
+      <c r="A73" s="89">
+        <v>1</v>
+      </c>
+      <c r="B73" s="40">
+        <v>6</v>
+      </c>
+      <c r="C73" s="39">
+        <v>4.2700000000000002E-2</v>
       </c>
       <c r="D73" s="61">
-        <v>0.1</v>
+        <v>4.2700000000000002E-2</v>
       </c>
       <c r="E73" s="61">
         <f t="shared" si="3"/>
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F73" s="59" t="s">
+        <v>1.8232900000000002E-3</v>
+      </c>
+      <c r="F73" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="58">
-        <v>1</v>
-      </c>
-      <c r="B74" s="59">
-        <v>7.5</v>
-      </c>
-      <c r="C74" s="60">
-        <v>9.5000000000000001E-2</v>
+    <row r="74" spans="1:6" s="90" customFormat="1">
+      <c r="A74" s="89">
+        <v>1</v>
+      </c>
+      <c r="B74" s="40">
+        <v>7</v>
+      </c>
+      <c r="C74" s="39">
+        <v>0.12720000000000001</v>
       </c>
       <c r="D74" s="61">
-        <v>0.12</v>
+        <v>0.12720000000000001</v>
       </c>
       <c r="E74" s="61">
         <f t="shared" si="3"/>
-        <v>1.14E-2</v>
-      </c>
-      <c r="F74" s="59" t="s">
+        <v>1.6179840000000001E-2</v>
+      </c>
+      <c r="F74" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="58">
-        <v>1</v>
-      </c>
-      <c r="B75" s="59">
+    <row r="75" spans="1:6" s="90" customFormat="1">
+      <c r="A75" s="89">
+        <v>1</v>
+      </c>
+      <c r="B75" s="40">
         <v>8</v>
       </c>
-      <c r="C75" s="60">
-        <v>0.1</v>
+      <c r="C75" s="39">
+        <v>0.2848</v>
       </c>
       <c r="D75" s="61">
-        <v>0.2</v>
+        <v>0.2848</v>
       </c>
       <c r="E75" s="61">
         <f t="shared" si="3"/>
-        <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="F75" s="59" t="s">
+        <v>8.1111039999999995E-2</v>
+      </c>
+      <c r="F75" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="58">
-        <v>1</v>
-      </c>
-      <c r="B76" s="59">
-        <v>8.5</v>
-      </c>
-      <c r="C76" s="60">
-        <v>0.11</v>
+    <row r="76" spans="1:6" s="90" customFormat="1">
+      <c r="A76" s="89">
+        <v>1</v>
+      </c>
+      <c r="B76" s="40">
+        <v>9</v>
+      </c>
+      <c r="C76" s="39">
+        <v>0.5</v>
       </c>
       <c r="D76" s="61">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="E76" s="61">
         <f t="shared" si="3"/>
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F76" s="59" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="F76" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="58">
-        <v>1</v>
-      </c>
-      <c r="B77" s="59">
-        <v>9</v>
-      </c>
-      <c r="C77" s="60">
-        <v>0.15</v>
+    <row r="77" spans="1:6" s="90" customFormat="1">
+      <c r="A77" s="89">
+        <v>1</v>
+      </c>
+      <c r="B77" s="40">
+        <v>10</v>
+      </c>
+      <c r="C77" s="39">
+        <v>0.71519999999999995</v>
       </c>
       <c r="D77" s="61">
-        <v>0.4</v>
+        <v>0.71519999999999995</v>
       </c>
       <c r="E77" s="61">
         <f t="shared" si="3"/>
-        <v>0.06</v>
-      </c>
-      <c r="F77" s="59" t="s">
+        <v>0.51151103999999992</v>
+      </c>
+      <c r="F77" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="58">
-        <v>1</v>
-      </c>
-      <c r="B78" s="59">
-        <v>9.5</v>
-      </c>
-      <c r="C78" s="60">
-        <v>0.159</v>
+    <row r="78" spans="1:6" s="90" customFormat="1">
+      <c r="A78" s="89">
+        <v>1</v>
+      </c>
+      <c r="B78" s="40">
+        <v>11</v>
+      </c>
+      <c r="C78" s="39">
+        <v>0.87280000000000002</v>
       </c>
       <c r="D78" s="61">
-        <v>0.43</v>
+        <v>0.87280000000000002</v>
       </c>
       <c r="E78" s="61">
         <f t="shared" si="3"/>
-        <v>6.837E-2</v>
-      </c>
-      <c r="F78" s="59" t="s">
+        <v>0.76177983999999999</v>
+      </c>
+      <c r="F78" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="58">
-        <v>1</v>
-      </c>
-      <c r="B79" s="59">
-        <v>10</v>
-      </c>
-      <c r="C79" s="60">
-        <v>0.2</v>
+    <row r="79" spans="1:6" s="90" customFormat="1">
+      <c r="A79" s="89">
+        <v>1</v>
+      </c>
+      <c r="B79" s="40">
+        <v>12</v>
+      </c>
+      <c r="C79" s="39">
+        <v>0.95730000000000004</v>
       </c>
       <c r="D79" s="61">
-        <v>0.45</v>
+        <v>0.95730000000000004</v>
       </c>
       <c r="E79" s="61">
         <f t="shared" si="3"/>
-        <v>9.0000000000000011E-2</v>
-      </c>
-      <c r="F79" s="59" t="s">
+        <v>0.91642329000000011</v>
+      </c>
+      <c r="F79" s="40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="58">
-        <v>1</v>
-      </c>
-      <c r="B80" s="59">
-        <v>10.5</v>
-      </c>
-      <c r="C80" s="60">
-        <v>0.23</v>
-      </c>
-      <c r="D80" s="61">
-        <v>0.47</v>
-      </c>
-      <c r="E80" s="61">
+    <row r="80" spans="1:6" s="90" customFormat="1">
+      <c r="A80" s="91">
+        <v>1</v>
+      </c>
+      <c r="B80" s="48">
+        <v>13</v>
+      </c>
+      <c r="C80" s="66">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="D80" s="65">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="E80" s="65">
         <f t="shared" si="3"/>
-        <v>0.1081</v>
-      </c>
-      <c r="F80" s="59" t="s">
+        <v>0.98109025000000005</v>
+      </c>
+      <c r="F80" s="48" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="58">
-        <v>1</v>
-      </c>
-      <c r="B81" s="59">
-        <v>11</v>
-      </c>
-      <c r="C81" s="60">
-        <v>0.27</v>
-      </c>
-      <c r="D81" s="61">
-        <v>0.49</v>
-      </c>
-      <c r="E81" s="61">
-        <f t="shared" si="3"/>
-        <v>0.1323</v>
-      </c>
-      <c r="F81" s="59" t="s">
-        <v>14</v>
+      <c r="A81" s="37">
+        <v>1</v>
+      </c>
+      <c r="B81" s="37">
+        <v>0</v>
+      </c>
+      <c r="C81" s="37">
+        <v>0</v>
+      </c>
+      <c r="D81" s="37">
+        <v>0</v>
+      </c>
+      <c r="E81" s="37">
+        <f>C81*D81</f>
+        <v>0</v>
+      </c>
+      <c r="F81" s="37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="58">
-        <v>1</v>
-      </c>
-      <c r="B82" s="59">
-        <v>11.5</v>
-      </c>
-      <c r="C82" s="60">
-        <v>0.31</v>
-      </c>
-      <c r="D82" s="61">
-        <v>0.5</v>
-      </c>
-      <c r="E82" s="61">
-        <f t="shared" si="3"/>
-        <v>0.155</v>
-      </c>
-      <c r="F82" s="59" t="s">
-        <v>14</v>
+      <c r="A82" s="37">
+        <v>1</v>
+      </c>
+      <c r="B82" s="37">
+        <v>10</v>
+      </c>
+      <c r="C82" s="37">
+        <v>0</v>
+      </c>
+      <c r="D82" s="37">
+        <v>0</v>
+      </c>
+      <c r="E82" s="37">
+        <f t="shared" ref="E82:E131" si="4">C82*D82</f>
+        <v>0</v>
+      </c>
+      <c r="F82" s="37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="58">
-        <v>1</v>
-      </c>
-      <c r="B83" s="59">
-        <v>12</v>
-      </c>
-      <c r="C83" s="60">
-        <v>0.38</v>
-      </c>
-      <c r="D83" s="61">
-        <v>0.51</v>
-      </c>
-      <c r="E83" s="61">
-        <f t="shared" si="3"/>
-        <v>0.1938</v>
-      </c>
-      <c r="F83" s="59" t="s">
-        <v>14</v>
+      <c r="A83" s="37">
+        <v>1</v>
+      </c>
+      <c r="B83" s="37">
+        <v>20</v>
+      </c>
+      <c r="C83" s="37">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="D83" s="37">
+        <v>1E-3</v>
+      </c>
+      <c r="E83" s="37">
+        <f t="shared" si="4"/>
+        <v>6.9999999999999997E-7</v>
+      </c>
+      <c r="F83" s="37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="58">
-        <v>1</v>
-      </c>
-      <c r="B84" s="59">
-        <v>12.5</v>
-      </c>
-      <c r="C84" s="60">
-        <v>0.39</v>
-      </c>
-      <c r="D84" s="61">
-        <v>0.52</v>
-      </c>
-      <c r="E84" s="61">
-        <f t="shared" si="3"/>
-        <v>0.20280000000000001</v>
-      </c>
-      <c r="F84" s="59" t="s">
-        <v>14</v>
+      <c r="A84" s="37">
+        <v>1</v>
+      </c>
+      <c r="B84" s="37">
+        <v>30</v>
+      </c>
+      <c r="C84" s="37">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D84" s="37">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E84" s="37">
+        <f t="shared" si="4"/>
+        <v>3.9099999999999998E-6</v>
+      </c>
+      <c r="F84" s="37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="62">
-        <v>1</v>
-      </c>
-      <c r="B85" s="63">
-        <v>13</v>
-      </c>
-      <c r="C85" s="64">
-        <v>0.4</v>
-      </c>
-      <c r="D85" s="65">
-        <v>0.53</v>
-      </c>
-      <c r="E85" s="65">
-        <f t="shared" si="3"/>
-        <v>0.21200000000000002</v>
-      </c>
-      <c r="F85" s="63" t="s">
-        <v>14</v>
+      <c r="A85" s="37">
+        <v>1</v>
+      </c>
+      <c r="B85" s="37">
+        <v>40</v>
+      </c>
+      <c r="C85" s="37">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="D85" s="37">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="E85" s="37">
+        <f t="shared" si="4"/>
+        <v>1.271E-5</v>
+      </c>
+      <c r="F85" s="37" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -4148,17 +4188,17 @@
         <v>1</v>
       </c>
       <c r="B86" s="37">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C86" s="37">
-        <v>0</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="D86" s="37">
-        <v>0</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="E86" s="37">
-        <f>C86*D86</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>3.0719999999999997E-5</v>
       </c>
       <c r="F86" s="37" t="s">
         <v>15</v>
@@ -4169,17 +4209,17 @@
         <v>1</v>
       </c>
       <c r="B87" s="37">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C87" s="37">
-        <v>0</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="D87" s="37">
-        <v>0</v>
+        <v>9.4999999999999998E-3</v>
       </c>
       <c r="E87" s="37">
-        <f t="shared" ref="E87:E136" si="4">C87*D87</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>6.745E-5</v>
       </c>
       <c r="F87" s="37" t="s">
         <v>15</v>
@@ -4190,17 +4230,17 @@
         <v>1</v>
       </c>
       <c r="B88" s="37">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C88" s="37">
-        <v>6.9999999999999999E-4</v>
+        <v>1.01E-2</v>
       </c>
       <c r="D88" s="37">
-        <v>1E-3</v>
+        <v>1.35E-2</v>
       </c>
       <c r="E88" s="37">
         <f t="shared" si="4"/>
-        <v>6.9999999999999997E-7</v>
+        <v>1.3634999999999998E-4</v>
       </c>
       <c r="F88" s="37" t="s">
         <v>15</v>
@@ -4211,17 +4251,17 @@
         <v>1</v>
       </c>
       <c r="B89" s="37">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C89" s="37">
-        <v>1.6999999999999999E-3</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="D89" s="37">
-        <v>2.3E-3</v>
+        <v>1.8599999999999998E-2</v>
       </c>
       <c r="E89" s="37">
         <f t="shared" si="4"/>
-        <v>3.9099999999999998E-6</v>
+        <v>2.5853999999999997E-4</v>
       </c>
       <c r="F89" s="37" t="s">
         <v>15</v>
@@ -4232,17 +4272,17 @@
         <v>1</v>
       </c>
       <c r="B90" s="37">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C90" s="37">
-        <v>3.0999999999999999E-3</v>
+        <v>1.8700000000000001E-2</v>
       </c>
       <c r="D90" s="37">
-        <v>4.1000000000000003E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E90" s="37">
         <f t="shared" si="4"/>
-        <v>1.271E-5</v>
+        <v>4.6750000000000003E-4</v>
       </c>
       <c r="F90" s="37" t="s">
         <v>15</v>
@@ -4253,17 +4293,17 @@
         <v>1</v>
       </c>
       <c r="B91" s="37">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C91" s="37">
-        <v>4.7999999999999996E-3</v>
+        <v>2.47E-2</v>
       </c>
       <c r="D91" s="37">
-        <v>6.4000000000000003E-3</v>
+        <v>3.2899999999999999E-2</v>
       </c>
       <c r="E91" s="37">
         <f t="shared" si="4"/>
-        <v>3.0719999999999997E-5</v>
+        <v>8.1262999999999995E-4</v>
       </c>
       <c r="F91" s="37" t="s">
         <v>15</v>
@@ -4274,17 +4314,17 @@
         <v>1</v>
       </c>
       <c r="B92" s="37">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C92" s="37">
-        <v>7.1000000000000004E-3</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D92" s="37">
-        <v>9.4999999999999998E-3</v>
+        <v>4.2700000000000002E-2</v>
       </c>
       <c r="E92" s="37">
         <f t="shared" si="4"/>
-        <v>6.745E-5</v>
+        <v>1.3664E-3</v>
       </c>
       <c r="F92" s="37" t="s">
         <v>15</v>
@@ -4295,17 +4335,17 @@
         <v>1</v>
       </c>
       <c r="B93" s="37">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C93" s="37">
-        <v>1.01E-2</v>
+        <v>4.0899999999999999E-2</v>
       </c>
       <c r="D93" s="37">
-        <v>1.35E-2</v>
+        <v>5.45E-2</v>
       </c>
       <c r="E93" s="37">
         <f t="shared" si="4"/>
-        <v>1.3634999999999998E-4</v>
+        <v>2.2290499999999998E-3</v>
       </c>
       <c r="F93" s="37" t="s">
         <v>15</v>
@@ -4316,17 +4356,17 @@
         <v>1</v>
       </c>
       <c r="B94" s="37">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C94" s="37">
-        <v>1.3899999999999999E-2</v>
+        <v>5.1499999999999997E-2</v>
       </c>
       <c r="D94" s="37">
-        <v>1.8599999999999998E-2</v>
+        <v>6.8699999999999997E-2</v>
       </c>
       <c r="E94" s="37">
         <f t="shared" si="4"/>
-        <v>2.5853999999999997E-4</v>
+        <v>3.5380499999999996E-3</v>
       </c>
       <c r="F94" s="37" t="s">
         <v>15</v>
@@ -4337,17 +4377,17 @@
         <v>1</v>
       </c>
       <c r="B95" s="37">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C95" s="37">
-        <v>1.8700000000000001E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D95" s="37">
-        <v>2.5000000000000001E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
       <c r="E95" s="37">
         <f t="shared" si="4"/>
-        <v>4.6750000000000003E-4</v>
+        <v>5.4592E-3</v>
       </c>
       <c r="F95" s="37" t="s">
         <v>15</v>
@@ -4358,17 +4398,17 @@
         <v>1</v>
       </c>
       <c r="B96" s="37">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C96" s="37">
-        <v>2.47E-2</v>
+        <v>7.8600000000000003E-2</v>
       </c>
       <c r="D96" s="37">
-        <v>3.2899999999999999E-2</v>
+        <v>0.1048</v>
       </c>
       <c r="E96" s="37">
         <f t="shared" si="4"/>
-        <v>8.1262999999999995E-4</v>
+        <v>8.2372800000000013E-3</v>
       </c>
       <c r="F96" s="37" t="s">
         <v>15</v>
@@ -4379,17 +4419,17 @@
         <v>1</v>
       </c>
       <c r="B97" s="37">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="C97" s="37">
-        <v>3.2000000000000001E-2</v>
+        <v>9.5399999999999999E-2</v>
       </c>
       <c r="D97" s="37">
-        <v>4.2700000000000002E-2</v>
+        <v>0.12720000000000001</v>
       </c>
       <c r="E97" s="37">
         <f t="shared" si="4"/>
-        <v>1.3664E-3</v>
+        <v>1.2134880000000001E-2</v>
       </c>
       <c r="F97" s="37" t="s">
         <v>15</v>
@@ -4400,17 +4440,17 @@
         <v>1</v>
       </c>
       <c r="B98" s="37">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="C98" s="37">
-        <v>4.0899999999999999E-2</v>
+        <v>0.1145</v>
       </c>
       <c r="D98" s="37">
-        <v>5.45E-2</v>
+        <v>0.1527</v>
       </c>
       <c r="E98" s="37">
         <f t="shared" si="4"/>
-        <v>2.2290499999999998E-3</v>
+        <v>1.748415E-2</v>
       </c>
       <c r="F98" s="37" t="s">
         <v>15</v>
@@ -4421,17 +4461,17 @@
         <v>1</v>
       </c>
       <c r="B99" s="37">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="C99" s="37">
-        <v>5.1499999999999997E-2</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="D99" s="37">
-        <v>6.8699999999999997E-2</v>
+        <v>0.1812</v>
       </c>
       <c r="E99" s="37">
         <f t="shared" si="4"/>
-        <v>3.5380499999999996E-3</v>
+        <v>2.4625079999999997E-2</v>
       </c>
       <c r="F99" s="37" t="s">
         <v>15</v>
@@ -4442,17 +4482,17 @@
         <v>1</v>
       </c>
       <c r="B100" s="37">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="C100" s="37">
-        <v>6.4000000000000001E-2</v>
+        <v>0.15959999999999999</v>
       </c>
       <c r="D100" s="37">
-        <v>8.5300000000000001E-2</v>
+        <v>0.21279999999999999</v>
       </c>
       <c r="E100" s="37">
         <f t="shared" si="4"/>
-        <v>5.4592E-3</v>
+        <v>3.3962879999999994E-2</v>
       </c>
       <c r="F100" s="37" t="s">
         <v>15</v>
@@ -4463,17 +4503,17 @@
         <v>1</v>
       </c>
       <c r="B101" s="37">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="C101" s="37">
-        <v>7.8600000000000003E-2</v>
+        <v>0.18559999999999999</v>
       </c>
       <c r="D101" s="37">
-        <v>0.1048</v>
+        <v>0.24740000000000001</v>
       </c>
       <c r="E101" s="37">
         <f t="shared" si="4"/>
-        <v>8.2372800000000013E-3</v>
+        <v>4.5917439999999997E-2</v>
       </c>
       <c r="F101" s="37" t="s">
         <v>15</v>
@@ -4484,17 +4524,17 @@
         <v>1</v>
       </c>
       <c r="B102" s="37">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="C102" s="37">
-        <v>9.5399999999999999E-2</v>
+        <v>0.21360000000000001</v>
       </c>
       <c r="D102" s="37">
-        <v>0.12720000000000001</v>
+        <v>0.2848</v>
       </c>
       <c r="E102" s="37">
         <f t="shared" si="4"/>
-        <v>1.2134880000000001E-2</v>
+        <v>6.0833280000000003E-2</v>
       </c>
       <c r="F102" s="37" t="s">
         <v>15</v>
@@ -4505,17 +4545,17 @@
         <v>1</v>
       </c>
       <c r="B103" s="37">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="C103" s="37">
-        <v>0.1145</v>
+        <v>0.24349999999999999</v>
       </c>
       <c r="D103" s="37">
-        <v>0.1527</v>
+        <v>0.3246</v>
       </c>
       <c r="E103" s="37">
         <f t="shared" si="4"/>
-        <v>1.748415E-2</v>
+        <v>7.9040100000000002E-2</v>
       </c>
       <c r="F103" s="37" t="s">
         <v>15</v>
@@ -4526,17 +4566,17 @@
         <v>1</v>
       </c>
       <c r="B104" s="37">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="C104" s="37">
-        <v>0.13589999999999999</v>
+        <v>0.27489999999999998</v>
       </c>
       <c r="D104" s="37">
-        <v>0.1812</v>
+        <v>0.36649999999999999</v>
       </c>
       <c r="E104" s="37">
         <f t="shared" si="4"/>
-        <v>2.4625079999999997E-2</v>
+        <v>0.10075084999999999</v>
       </c>
       <c r="F104" s="37" t="s">
         <v>15</v>
@@ -4547,17 +4587,17 @@
         <v>1</v>
       </c>
       <c r="B105" s="37">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="C105" s="37">
-        <v>0.15959999999999999</v>
+        <v>0.30759999999999998</v>
       </c>
       <c r="D105" s="37">
-        <v>0.21279999999999999</v>
+        <v>0.41010000000000002</v>
       </c>
       <c r="E105" s="37">
         <f t="shared" si="4"/>
-        <v>3.3962879999999994E-2</v>
+        <v>0.12614676</v>
       </c>
       <c r="F105" s="37" t="s">
         <v>15</v>
@@ -4568,17 +4608,17 @@
         <v>1</v>
       </c>
       <c r="B106" s="37">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="C106" s="37">
-        <v>0.18559999999999999</v>
+        <v>0.34110000000000001</v>
       </c>
       <c r="D106" s="37">
-        <v>0.24740000000000001</v>
+        <v>0.45469999999999999</v>
       </c>
       <c r="E106" s="37">
         <f t="shared" si="4"/>
-        <v>4.5917439999999997E-2</v>
+        <v>0.15509817000000001</v>
       </c>
       <c r="F106" s="37" t="s">
         <v>15</v>
@@ -4589,17 +4629,17 @@
         <v>1</v>
       </c>
       <c r="B107" s="37">
-        <v>210</v>
+        <v>260</v>
       </c>
       <c r="C107" s="37">
-        <v>0.21360000000000001</v>
+        <v>0.375</v>
       </c>
       <c r="D107" s="37">
-        <v>0.2848</v>
+        <v>0.5</v>
       </c>
       <c r="E107" s="37">
         <f t="shared" si="4"/>
-        <v>6.0833280000000003E-2</v>
+        <v>0.1875</v>
       </c>
       <c r="F107" s="37" t="s">
         <v>15</v>
@@ -4610,17 +4650,17 @@
         <v>1</v>
       </c>
       <c r="B108" s="37">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="C108" s="37">
-        <v>0.24349999999999999</v>
+        <v>0.40889999999999999</v>
       </c>
       <c r="D108" s="37">
-        <v>0.3246</v>
+        <v>0.54530000000000001</v>
       </c>
       <c r="E108" s="37">
         <f t="shared" si="4"/>
-        <v>7.9040100000000002E-2</v>
+        <v>0.22297317</v>
       </c>
       <c r="F108" s="37" t="s">
         <v>15</v>
@@ -4631,17 +4671,17 @@
         <v>1</v>
       </c>
       <c r="B109" s="37">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="C109" s="37">
-        <v>0.27489999999999998</v>
+        <v>0.44240000000000002</v>
       </c>
       <c r="D109" s="37">
-        <v>0.36649999999999999</v>
+        <v>0.58989999999999998</v>
       </c>
       <c r="E109" s="37">
         <f t="shared" si="4"/>
-        <v>0.10075084999999999</v>
+        <v>0.26097176</v>
       </c>
       <c r="F109" s="37" t="s">
         <v>15</v>
@@ -4652,17 +4692,17 @@
         <v>1</v>
       </c>
       <c r="B110" s="37">
-        <v>240</v>
+        <v>290</v>
       </c>
       <c r="C110" s="37">
-        <v>0.30759999999999998</v>
+        <v>0.47510000000000002</v>
       </c>
       <c r="D110" s="37">
-        <v>0.41010000000000002</v>
+        <v>0.63349999999999995</v>
       </c>
       <c r="E110" s="37">
         <f t="shared" si="4"/>
-        <v>0.12614676</v>
+        <v>0.30097584999999999</v>
       </c>
       <c r="F110" s="37" t="s">
         <v>15</v>
@@ -4673,17 +4713,17 @@
         <v>1</v>
       </c>
       <c r="B111" s="37">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C111" s="37">
-        <v>0.34110000000000001</v>
+        <v>0.50649999999999995</v>
       </c>
       <c r="D111" s="37">
-        <v>0.45469999999999999</v>
+        <v>0.6754</v>
       </c>
       <c r="E111" s="37">
         <f t="shared" si="4"/>
-        <v>0.15509817000000001</v>
+        <v>0.34209009999999995</v>
       </c>
       <c r="F111" s="37" t="s">
         <v>15</v>
@@ -4694,17 +4734,17 @@
         <v>1</v>
       </c>
       <c r="B112" s="37">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="C112" s="37">
-        <v>0.375</v>
+        <v>0.53639999999999999</v>
       </c>
       <c r="D112" s="37">
-        <v>0.5</v>
+        <v>0.71519999999999995</v>
       </c>
       <c r="E112" s="37">
         <f t="shared" si="4"/>
-        <v>0.1875</v>
+        <v>0.38363327999999997</v>
       </c>
       <c r="F112" s="37" t="s">
         <v>15</v>
@@ -4715,17 +4755,17 @@
         <v>1</v>
       </c>
       <c r="B113" s="37">
-        <v>270</v>
+        <v>320</v>
       </c>
       <c r="C113" s="37">
-        <v>0.40889999999999999</v>
+        <v>0.56440000000000001</v>
       </c>
       <c r="D113" s="37">
-        <v>0.54530000000000001</v>
+        <v>0.75260000000000005</v>
       </c>
       <c r="E113" s="37">
         <f t="shared" si="4"/>
-        <v>0.22297317</v>
+        <v>0.42476744000000005</v>
       </c>
       <c r="F113" s="37" t="s">
         <v>15</v>
@@ -4736,17 +4776,17 @@
         <v>1</v>
       </c>
       <c r="B114" s="37">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="C114" s="37">
-        <v>0.44240000000000002</v>
+        <v>0.59040000000000004</v>
       </c>
       <c r="D114" s="37">
-        <v>0.58989999999999998</v>
+        <v>0.78720000000000001</v>
       </c>
       <c r="E114" s="37">
         <f t="shared" si="4"/>
-        <v>0.26097176</v>
+        <v>0.46476288000000004</v>
       </c>
       <c r="F114" s="37" t="s">
         <v>15</v>
@@ -4757,17 +4797,17 @@
         <v>1</v>
       </c>
       <c r="B115" s="37">
-        <v>290</v>
+        <v>340</v>
       </c>
       <c r="C115" s="37">
-        <v>0.47510000000000002</v>
+        <v>0.61409999999999998</v>
       </c>
       <c r="D115" s="37">
-        <v>0.63349999999999995</v>
+        <v>0.81879999999999997</v>
       </c>
       <c r="E115" s="37">
         <f t="shared" si="4"/>
-        <v>0.30097584999999999</v>
+        <v>0.50282507999999992</v>
       </c>
       <c r="F115" s="37" t="s">
         <v>15</v>
@@ -4778,17 +4818,17 @@
         <v>1</v>
       </c>
       <c r="B116" s="37">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="C116" s="37">
-        <v>0.50649999999999995</v>
+        <v>0.63549999999999995</v>
       </c>
       <c r="D116" s="37">
-        <v>0.6754</v>
+        <v>0.84730000000000005</v>
       </c>
       <c r="E116" s="37">
         <f t="shared" si="4"/>
-        <v>0.34209009999999995</v>
+        <v>0.53845915</v>
       </c>
       <c r="F116" s="37" t="s">
         <v>15</v>
@@ -4799,17 +4839,17 @@
         <v>1</v>
       </c>
       <c r="B117" s="37">
-        <v>310</v>
+        <v>360</v>
       </c>
       <c r="C117" s="37">
-        <v>0.53639999999999999</v>
+        <v>0.65459999999999996</v>
       </c>
       <c r="D117" s="37">
-        <v>0.71519999999999995</v>
+        <v>0.87280000000000002</v>
       </c>
       <c r="E117" s="37">
         <f t="shared" si="4"/>
-        <v>0.38363327999999997</v>
+        <v>0.57133487999999999</v>
       </c>
       <c r="F117" s="37" t="s">
         <v>15</v>
@@ -4820,17 +4860,17 @@
         <v>1</v>
       </c>
       <c r="B118" s="37">
-        <v>320</v>
+        <v>370</v>
       </c>
       <c r="C118" s="37">
-        <v>0.56440000000000001</v>
+        <v>0.6714</v>
       </c>
       <c r="D118" s="37">
-        <v>0.75260000000000005</v>
+        <v>0.8952</v>
       </c>
       <c r="E118" s="37">
         <f t="shared" si="4"/>
-        <v>0.42476744000000005</v>
+        <v>0.60103728000000001</v>
       </c>
       <c r="F118" s="37" t="s">
         <v>15</v>
@@ -4841,17 +4881,17 @@
         <v>1</v>
       </c>
       <c r="B119" s="37">
-        <v>330</v>
+        <v>380</v>
       </c>
       <c r="C119" s="37">
-        <v>0.59040000000000004</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="D119" s="37">
-        <v>0.78720000000000001</v>
+        <v>0.91469999999999996</v>
       </c>
       <c r="E119" s="37">
         <f t="shared" si="4"/>
-        <v>0.46476288000000004</v>
+        <v>0.62748420000000005</v>
       </c>
       <c r="F119" s="37" t="s">
         <v>15</v>
@@ -4862,17 +4902,17 @@
         <v>1</v>
       </c>
       <c r="B120" s="37">
-        <v>340</v>
+        <v>390</v>
       </c>
       <c r="C120" s="37">
-        <v>0.61409999999999998</v>
+        <v>0.69850000000000001</v>
       </c>
       <c r="D120" s="37">
-        <v>0.81879999999999997</v>
+        <v>0.93130000000000002</v>
       </c>
       <c r="E120" s="37">
         <f t="shared" si="4"/>
-        <v>0.50282507999999992</v>
+        <v>0.65051305000000004</v>
       </c>
       <c r="F120" s="37" t="s">
         <v>15</v>
@@ -4883,17 +4923,17 @@
         <v>1</v>
       </c>
       <c r="B121" s="37">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="C121" s="37">
-        <v>0.63549999999999995</v>
+        <v>0.70909999999999995</v>
       </c>
       <c r="D121" s="37">
-        <v>0.84730000000000005</v>
+        <v>0.94550000000000001</v>
       </c>
       <c r="E121" s="37">
         <f t="shared" si="4"/>
-        <v>0.53845915</v>
+        <v>0.67045404999999991</v>
       </c>
       <c r="F121" s="37" t="s">
         <v>15</v>
@@ -4904,17 +4944,17 @@
         <v>1</v>
       </c>
       <c r="B122" s="37">
-        <v>360</v>
+        <v>410</v>
       </c>
       <c r="C122" s="37">
-        <v>0.65459999999999996</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="D122" s="37">
-        <v>0.87280000000000002</v>
+        <v>0.95730000000000004</v>
       </c>
       <c r="E122" s="37">
         <f t="shared" si="4"/>
-        <v>0.57133487999999999</v>
+        <v>0.68734139999999999</v>
       </c>
       <c r="F122" s="37" t="s">
         <v>15</v>
@@ -4925,17 +4965,17 @@
         <v>1</v>
       </c>
       <c r="B123" s="37">
-        <v>370</v>
+        <v>420</v>
       </c>
       <c r="C123" s="37">
-        <v>0.6714</v>
+        <v>0.72529999999999994</v>
       </c>
       <c r="D123" s="37">
-        <v>0.8952</v>
+        <v>0.96709999999999996</v>
       </c>
       <c r="E123" s="37">
         <f t="shared" si="4"/>
-        <v>0.60103728000000001</v>
+        <v>0.70143762999999992</v>
       </c>
       <c r="F123" s="37" t="s">
         <v>15</v>
@@ -4946,17 +4986,17 @@
         <v>1</v>
       </c>
       <c r="B124" s="37">
-        <v>380</v>
+        <v>430</v>
       </c>
       <c r="C124" s="37">
-        <v>0.68600000000000005</v>
+        <v>0.73129999999999995</v>
       </c>
       <c r="D124" s="37">
-        <v>0.91469999999999996</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E124" s="37">
         <f t="shared" si="4"/>
-        <v>0.62748420000000005</v>
+        <v>0.71301749999999997</v>
       </c>
       <c r="F124" s="37" t="s">
         <v>15</v>
@@ -4967,17 +5007,17 @@
         <v>1</v>
       </c>
       <c r="B125" s="37">
-        <v>390</v>
+        <v>440</v>
       </c>
       <c r="C125" s="37">
-        <v>0.69850000000000001</v>
+        <v>0.73609999999999998</v>
       </c>
       <c r="D125" s="37">
-        <v>0.93130000000000002</v>
+        <v>0.98140000000000005</v>
       </c>
       <c r="E125" s="37">
         <f t="shared" si="4"/>
-        <v>0.65051305000000004</v>
+        <v>0.72240853999999999</v>
       </c>
       <c r="F125" s="37" t="s">
         <v>15</v>
@@ -4988,17 +5028,17 @@
         <v>1</v>
       </c>
       <c r="B126" s="37">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="C126" s="37">
-        <v>0.70909999999999995</v>
+        <v>0.7399</v>
       </c>
       <c r="D126" s="37">
-        <v>0.94550000000000001</v>
+        <v>0.98650000000000004</v>
       </c>
       <c r="E126" s="37">
         <f t="shared" si="4"/>
-        <v>0.67045404999999991</v>
+        <v>0.72991135000000007</v>
       </c>
       <c r="F126" s="37" t="s">
         <v>15</v>
@@ -5009,17 +5049,17 @@
         <v>1</v>
       </c>
       <c r="B127" s="37">
-        <v>410</v>
+        <v>460</v>
       </c>
       <c r="C127" s="37">
-        <v>0.71799999999999997</v>
+        <v>0.7429</v>
       </c>
       <c r="D127" s="37">
-        <v>0.95730000000000004</v>
+        <v>0.99050000000000005</v>
       </c>
       <c r="E127" s="37">
         <f t="shared" si="4"/>
-        <v>0.68734139999999999</v>
+        <v>0.73584245000000004</v>
       </c>
       <c r="F127" s="37" t="s">
         <v>15</v>
@@ -5030,17 +5070,17 @@
         <v>1</v>
       </c>
       <c r="B128" s="37">
-        <v>420</v>
+        <v>470</v>
       </c>
       <c r="C128" s="37">
-        <v>0.72529999999999994</v>
+        <v>0.74519999999999997</v>
       </c>
       <c r="D128" s="37">
-        <v>0.96709999999999996</v>
+        <v>0.99360000000000004</v>
       </c>
       <c r="E128" s="37">
         <f t="shared" si="4"/>
-        <v>0.70143762999999992</v>
+        <v>0.74043071999999999</v>
       </c>
       <c r="F128" s="37" t="s">
         <v>15</v>
@@ -5051,17 +5091,17 @@
         <v>1</v>
       </c>
       <c r="B129" s="37">
-        <v>430</v>
+        <v>480</v>
       </c>
       <c r="C129" s="37">
-        <v>0.73129999999999995</v>
+        <v>0.74690000000000001</v>
       </c>
       <c r="D129" s="37">
-        <v>0.97499999999999998</v>
+        <v>0.99590000000000001</v>
       </c>
       <c r="E129" s="37">
         <f t="shared" si="4"/>
-        <v>0.71301749999999997</v>
+        <v>0.74383770999999999</v>
       </c>
       <c r="F129" s="37" t="s">
         <v>15</v>
@@ -5072,146 +5112,629 @@
         <v>1</v>
       </c>
       <c r="B130" s="37">
-        <v>440</v>
+        <v>490</v>
       </c>
       <c r="C130" s="37">
-        <v>0.73609999999999998</v>
+        <v>0.74829999999999997</v>
       </c>
       <c r="D130" s="37">
-        <v>0.98140000000000005</v>
+        <v>0.99770000000000003</v>
       </c>
       <c r="E130" s="37">
         <f t="shared" si="4"/>
-        <v>0.72240853999999999</v>
+        <v>0.74657890999999998</v>
       </c>
       <c r="F130" s="37" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:6">
-      <c r="A131" s="37">
-        <v>1</v>
-      </c>
-      <c r="B131" s="37">
-        <v>450</v>
-      </c>
-      <c r="C131" s="37">
-        <v>0.7399</v>
-      </c>
-      <c r="D131" s="37">
-        <v>0.98650000000000004</v>
-      </c>
-      <c r="E131" s="37">
-        <f t="shared" si="4"/>
-        <v>0.72991135000000007</v>
-      </c>
-      <c r="F131" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="37">
-        <v>1</v>
-      </c>
-      <c r="B132" s="37">
-        <v>460</v>
-      </c>
-      <c r="C132" s="37">
-        <v>0.7429</v>
-      </c>
-      <c r="D132" s="37">
-        <v>0.99050000000000005</v>
-      </c>
-      <c r="E132" s="37">
-        <f t="shared" si="4"/>
-        <v>0.73584245000000004</v>
-      </c>
-      <c r="F132" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="37">
-        <v>1</v>
-      </c>
-      <c r="B133" s="37">
-        <v>470</v>
-      </c>
-      <c r="C133" s="37">
-        <v>0.74519999999999997</v>
-      </c>
-      <c r="D133" s="37">
-        <v>0.99360000000000004</v>
-      </c>
-      <c r="E133" s="37">
-        <f t="shared" si="4"/>
-        <v>0.74043071999999999</v>
-      </c>
-      <c r="F133" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="37">
-        <v>1</v>
-      </c>
-      <c r="B134" s="37">
-        <v>480</v>
-      </c>
-      <c r="C134" s="37">
-        <v>0.74690000000000001</v>
-      </c>
-      <c r="D134" s="37">
-        <v>0.99590000000000001</v>
-      </c>
-      <c r="E134" s="37">
-        <f t="shared" si="4"/>
-        <v>0.74383770999999999</v>
-      </c>
-      <c r="F134" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="37">
-        <v>1</v>
-      </c>
-      <c r="B135" s="37">
-        <v>490</v>
-      </c>
-      <c r="C135" s="37">
-        <v>0.74829999999999997</v>
-      </c>
-      <c r="D135" s="37">
-        <v>0.99770000000000003</v>
-      </c>
-      <c r="E135" s="37">
-        <f t="shared" si="4"/>
-        <v>0.74657890999999998</v>
-      </c>
-      <c r="F135" s="37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="78">
-        <v>1</v>
-      </c>
-      <c r="B136" s="78">
+      <c r="A131" s="78">
+        <v>1</v>
+      </c>
+      <c r="B131" s="78">
         <v>500</v>
       </c>
-      <c r="C136" s="78">
+      <c r="C131" s="78">
         <v>0.74929999999999997</v>
       </c>
-      <c r="D136" s="78">
+      <c r="D131" s="78">
         <v>0.999</v>
       </c>
-      <c r="E136" s="78">
+      <c r="E131" s="78">
         <f t="shared" si="4"/>
         <v>0.74855070000000001</v>
       </c>
-      <c r="F136" s="78" t="s">
+      <c r="F131" s="78" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="92">
+        <v>1</v>
+      </c>
+      <c r="B132" s="92">
+        <v>0</v>
+      </c>
+      <c r="C132" s="92">
+        <v>0</v>
+      </c>
+      <c r="D132" s="92">
+        <v>0</v>
+      </c>
+      <c r="E132" s="92">
+        <f>C132*D132</f>
+        <v>0</v>
+      </c>
+      <c r="F132" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="92">
+        <v>1</v>
+      </c>
+      <c r="B133" s="92">
+        <v>50</v>
+      </c>
+      <c r="C133" s="92">
+        <v>0</v>
+      </c>
+      <c r="D133" s="92">
+        <v>0</v>
+      </c>
+      <c r="E133" s="92">
+        <f t="shared" ref="E133:E159" si="5">C133*D133</f>
+        <v>0</v>
+      </c>
+      <c r="F133" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="92">
+        <v>1</v>
+      </c>
+      <c r="B134" s="92">
+        <v>100</v>
+      </c>
+      <c r="C134" s="92">
+        <v>0</v>
+      </c>
+      <c r="D134" s="92">
+        <v>0</v>
+      </c>
+      <c r="E134" s="92">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F134" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="92">
+        <v>1</v>
+      </c>
+      <c r="B135" s="92">
+        <v>150</v>
+      </c>
+      <c r="C135" s="92">
+        <v>0</v>
+      </c>
+      <c r="D135" s="92">
+        <v>0</v>
+      </c>
+      <c r="E135" s="92">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F135" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="92">
+        <v>1</v>
+      </c>
+      <c r="B136" s="92">
+        <v>200</v>
+      </c>
+      <c r="C136" s="92">
+        <v>0</v>
+      </c>
+      <c r="D136" s="92">
+        <v>0</v>
+      </c>
+      <c r="E136" s="92">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F136" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="92">
+        <v>1</v>
+      </c>
+      <c r="B137" s="92">
+        <v>250</v>
+      </c>
+      <c r="C137" s="92">
+        <v>0</v>
+      </c>
+      <c r="D137" s="92">
+        <v>0</v>
+      </c>
+      <c r="E137" s="92">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F137" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="92">
+        <v>1</v>
+      </c>
+      <c r="B138" s="92">
+        <v>300</v>
+      </c>
+      <c r="C138" s="92">
+        <v>0</v>
+      </c>
+      <c r="D138" s="92">
+        <v>0</v>
+      </c>
+      <c r="E138" s="92">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F138" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="92">
+        <v>1</v>
+      </c>
+      <c r="B139" s="92">
+        <v>350</v>
+      </c>
+      <c r="C139" s="92">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="D139" s="92">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="E139" s="92">
+        <f t="shared" si="5"/>
+        <v>4.4199999999999992E-6</v>
+      </c>
+      <c r="F139" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="92">
+        <v>1</v>
+      </c>
+      <c r="B140" s="92">
+        <v>400</v>
+      </c>
+      <c r="C140" s="92">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="D140" s="92">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="E140" s="92">
+        <f t="shared" si="5"/>
+        <v>4.0949999999999999E-5</v>
+      </c>
+      <c r="F140" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="92">
+        <v>1</v>
+      </c>
+      <c r="B141" s="92">
+        <v>450</v>
+      </c>
+      <c r="C141" s="92">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="D141" s="92">
+        <v>2.4299999999999999E-2</v>
+      </c>
+      <c r="E141" s="92">
+        <f t="shared" si="5"/>
+        <v>2.2112999999999999E-4</v>
+      </c>
+      <c r="F141" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="92">
+        <v>1</v>
+      </c>
+      <c r="B142" s="92">
+        <v>500</v>
+      </c>
+      <c r="C142" s="92">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="D142" s="92">
+        <v>4.87E-2</v>
+      </c>
+      <c r="E142" s="92">
+        <f t="shared" si="5"/>
+        <v>8.8634E-4</v>
+      </c>
+      <c r="F142" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="92">
+        <v>1</v>
+      </c>
+      <c r="B143" s="92">
+        <v>550</v>
+      </c>
+      <c r="C143" s="92">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="D143" s="92">
+        <v>8.8200000000000001E-2</v>
+      </c>
+      <c r="E143" s="92">
+        <f t="shared" si="5"/>
+        <v>2.9194199999999998E-3</v>
+      </c>
+      <c r="F143" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="92">
+        <v>1</v>
+      </c>
+      <c r="B144" s="92">
+        <v>600</v>
+      </c>
+      <c r="C144" s="92">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="D144" s="92">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="E144" s="92">
+        <f t="shared" si="5"/>
+        <v>8.0996999999999996E-3</v>
+      </c>
+      <c r="F144" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="92">
+        <v>1</v>
+      </c>
+      <c r="B145" s="92">
+        <v>650</v>
+      </c>
+      <c r="C145" s="92">
+        <v>8.5099999999999995E-2</v>
+      </c>
+      <c r="D145" s="92">
+        <v>0.2271</v>
+      </c>
+      <c r="E145" s="92">
+        <f t="shared" si="5"/>
+        <v>1.932621E-2</v>
+      </c>
+      <c r="F145" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="92">
+        <v>1</v>
+      </c>
+      <c r="B146" s="92">
+        <v>700</v>
+      </c>
+      <c r="C146" s="92">
+        <v>0.1225</v>
+      </c>
+      <c r="D146" s="92">
+        <v>0.32679999999999998</v>
+      </c>
+      <c r="E146" s="92">
+        <f t="shared" si="5"/>
+        <v>4.0032999999999999E-2</v>
+      </c>
+      <c r="F146" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="92">
+        <v>1</v>
+      </c>
+      <c r="B147" s="92">
+        <v>750</v>
+      </c>
+      <c r="C147" s="92">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="D147" s="92">
+        <v>0.44059999999999999</v>
+      </c>
+      <c r="E147" s="92">
+        <f t="shared" si="5"/>
+        <v>7.2787120000000011E-2</v>
+      </c>
+      <c r="F147" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="92">
+        <v>1</v>
+      </c>
+      <c r="B148" s="92">
+        <v>800</v>
+      </c>
+      <c r="C148" s="92">
+        <v>0.20979999999999999</v>
+      </c>
+      <c r="D148" s="92">
+        <v>0.55940000000000001</v>
+      </c>
+      <c r="E148" s="92">
+        <f t="shared" si="5"/>
+        <v>0.11736212</v>
+      </c>
+      <c r="F148" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="92">
+        <v>1</v>
+      </c>
+      <c r="B149" s="92">
+        <v>850</v>
+      </c>
+      <c r="C149" s="92">
+        <v>0.2525</v>
+      </c>
+      <c r="D149" s="92">
+        <v>0.67320000000000002</v>
+      </c>
+      <c r="E149" s="92">
+        <f t="shared" si="5"/>
+        <v>0.169983</v>
+      </c>
+      <c r="F149" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="92">
+        <v>1</v>
+      </c>
+      <c r="B150" s="92">
+        <v>900</v>
+      </c>
+      <c r="C150" s="92">
+        <v>0.28989999999999999</v>
+      </c>
+      <c r="D150" s="92">
+        <v>0.77290000000000003</v>
+      </c>
+      <c r="E150" s="92">
+        <f t="shared" si="5"/>
+        <v>0.22406371</v>
+      </c>
+      <c r="F150" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="92">
+        <v>1</v>
+      </c>
+      <c r="B151" s="92">
+        <v>950</v>
+      </c>
+      <c r="C151" s="92">
+        <v>0.31990000000000002</v>
+      </c>
+      <c r="D151" s="92">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="E151" s="92">
+        <f t="shared" si="5"/>
+        <v>0.27287470000000003</v>
+      </c>
+      <c r="F151" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="92">
+        <v>1</v>
+      </c>
+      <c r="B152" s="92">
+        <v>1000</v>
+      </c>
+      <c r="C152" s="92">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="D152" s="92">
+        <v>0.91180000000000005</v>
+      </c>
+      <c r="E152" s="92">
+        <f t="shared" si="5"/>
+        <v>0.31174442000000002</v>
+      </c>
+      <c r="F152" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="92">
+        <v>1</v>
+      </c>
+      <c r="B153" s="92">
+        <v>1050</v>
+      </c>
+      <c r="C153" s="92">
+        <v>0.35680000000000001</v>
+      </c>
+      <c r="D153" s="92">
+        <v>0.95130000000000003</v>
+      </c>
+      <c r="E153" s="92">
+        <f t="shared" si="5"/>
+        <v>0.33942384000000003</v>
+      </c>
+      <c r="F153" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="92">
+        <v>1</v>
+      </c>
+      <c r="B154" s="92">
+        <v>1100</v>
+      </c>
+      <c r="C154" s="92">
+        <v>0.3659</v>
+      </c>
+      <c r="D154" s="92">
+        <v>0.97570000000000001</v>
+      </c>
+      <c r="E154" s="92">
+        <f t="shared" si="5"/>
+        <v>0.35700862999999999</v>
+      </c>
+      <c r="F154" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="92">
+        <v>1</v>
+      </c>
+      <c r="B155" s="92">
+        <v>1150</v>
+      </c>
+      <c r="C155" s="92">
+        <v>0.37109999999999999</v>
+      </c>
+      <c r="D155" s="92">
+        <v>0.98950000000000005</v>
+      </c>
+      <c r="E155" s="92">
+        <f t="shared" si="5"/>
+        <v>0.36720344999999999</v>
+      </c>
+      <c r="F155" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="92">
+        <v>1</v>
+      </c>
+      <c r="B156" s="92">
+        <v>1200</v>
+      </c>
+      <c r="C156" s="92">
+        <v>0.37369999999999998</v>
+      </c>
+      <c r="D156" s="92">
+        <v>0.99660000000000004</v>
+      </c>
+      <c r="E156" s="92">
+        <f t="shared" si="5"/>
+        <v>0.37242942000000001</v>
+      </c>
+      <c r="F156" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="92">
+        <v>1</v>
+      </c>
+      <c r="B157" s="92">
+        <v>1500</v>
+      </c>
+      <c r="C157" s="92">
+        <v>0.37369999999999998</v>
+      </c>
+      <c r="D157" s="92">
+        <v>0.99660000000000004</v>
+      </c>
+      <c r="E157" s="92">
+        <f t="shared" si="5"/>
+        <v>0.37242942000000001</v>
+      </c>
+      <c r="F157" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="92">
+        <v>1</v>
+      </c>
+      <c r="B158" s="92">
+        <v>2000</v>
+      </c>
+      <c r="C158" s="92">
+        <v>0.37369999999999998</v>
+      </c>
+      <c r="D158" s="92">
+        <v>0.99660000000000004</v>
+      </c>
+      <c r="E158" s="92">
+        <f t="shared" si="5"/>
+        <v>0.37242942000000001</v>
+      </c>
+      <c r="F158" s="92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="93">
+        <v>1</v>
+      </c>
+      <c r="B159" s="93">
+        <v>3000</v>
+      </c>
+      <c r="C159" s="93">
+        <v>0.37369999999999998</v>
+      </c>
+      <c r="D159" s="93">
+        <v>0.99660000000000004</v>
+      </c>
+      <c r="E159" s="93">
+        <f t="shared" si="5"/>
+        <v>0.37242942000000001</v>
+      </c>
+      <c r="F159" s="93" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -5230,7 +5753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
hazard plot improved (further ;-)
dummy FL damage function (same as TS) added in entity_template
</commit_message>
<xml_diff>
--- a/data/entities/entity_template.xlsx
+++ b/data/entities/entity_template.xlsx
@@ -161,6 +161,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>A satisfied Microsoft Office user</author>
+    <author>David N. Bresch</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -420,6 +421,32 @@
             <rFont val="Calibri"/>
           </rPr>
           <t>o show the effect, NOT a really good damage function.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A238" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">added 20141204
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F238" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">20160929, added dummy FL damage function, a copy of TS
+</t>
         </r>
       </text>
     </comment>
@@ -780,7 +807,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="110">
   <si>
     <t>Category_ID</t>
   </si>
@@ -1173,6 +1200,12 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Flood default</t>
   </si>
 </sst>
 </file>
@@ -2632,10 +2665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H237"/>
+  <dimension ref="A1:H256"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132:G159"/>
+      <selection activeCell="I243" sqref="I243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.33203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -9037,6 +9070,519 @@
       </c>
       <c r="H237" s="82" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A238" s="32">
+        <v>1</v>
+      </c>
+      <c r="B238" s="32">
+        <v>0</v>
+      </c>
+      <c r="C238" s="33">
+        <v>0</v>
+      </c>
+      <c r="D238" s="33">
+        <v>0</v>
+      </c>
+      <c r="E238" s="33">
+        <f>C238*D238</f>
+        <v>0</v>
+      </c>
+      <c r="F238" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G238" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H238" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A239" s="32">
+        <v>1</v>
+      </c>
+      <c r="B239" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="C239" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D239" s="33">
+        <v>0.39346934028736658</v>
+      </c>
+      <c r="E239" s="33">
+        <f t="shared" ref="E239:E254" si="7">C239*D239</f>
+        <v>3.9346934028736662E-3</v>
+      </c>
+      <c r="F239" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G239" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H239" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A240" s="32">
+        <v>1</v>
+      </c>
+      <c r="B240" s="32">
+        <v>1</v>
+      </c>
+      <c r="C240" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D240" s="33">
+        <v>0.63212055882855767</v>
+      </c>
+      <c r="E240" s="33">
+        <f t="shared" si="7"/>
+        <v>1.2642411176571153E-2</v>
+      </c>
+      <c r="F240" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G240" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H240" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A241" s="32">
+        <v>1</v>
+      </c>
+      <c r="B241" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="C241" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="D241" s="33">
+        <v>0.77686983985157021</v>
+      </c>
+      <c r="E241" s="33">
+        <f t="shared" si="7"/>
+        <v>3.8843491992578513E-2</v>
+      </c>
+      <c r="F241" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G241" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H241" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A242" s="32">
+        <v>1</v>
+      </c>
+      <c r="B242" s="32">
+        <v>2</v>
+      </c>
+      <c r="C242" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="D242" s="33">
+        <v>0.8646647167633873</v>
+      </c>
+      <c r="E242" s="33">
+        <f t="shared" si="7"/>
+        <v>8.6466471676338738E-2</v>
+      </c>
+      <c r="F242" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G242" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H242" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A243" s="32">
+        <v>1</v>
+      </c>
+      <c r="B243" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="C243" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="D243" s="33">
+        <v>0.91791500137610116</v>
+      </c>
+      <c r="E243" s="33">
+        <f t="shared" si="7"/>
+        <v>0.18358300027522023</v>
+      </c>
+      <c r="F243" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G243" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H243" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A244" s="32">
+        <v>1</v>
+      </c>
+      <c r="B244" s="32">
+        <v>3</v>
+      </c>
+      <c r="C244" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="D244" s="33">
+        <v>0.95021293163213605</v>
+      </c>
+      <c r="E244" s="33">
+        <f t="shared" si="7"/>
+        <v>0.28506387948964079</v>
+      </c>
+      <c r="F244" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G244" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H244" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A245" s="32">
+        <v>1</v>
+      </c>
+      <c r="B245" s="32">
+        <v>3.5</v>
+      </c>
+      <c r="C245" s="33">
+        <v>0.4</v>
+      </c>
+      <c r="D245" s="33">
+        <v>0.96980261657768152</v>
+      </c>
+      <c r="E245" s="33">
+        <f t="shared" si="7"/>
+        <v>0.38792104663107263</v>
+      </c>
+      <c r="F245" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G245" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H245" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A246" s="32">
+        <v>1</v>
+      </c>
+      <c r="B246" s="32">
+        <v>4</v>
+      </c>
+      <c r="C246" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="D246" s="33">
+        <v>0.98168436111126578</v>
+      </c>
+      <c r="E246" s="33">
+        <f t="shared" si="7"/>
+        <v>0.49084218055563289</v>
+      </c>
+      <c r="F246" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G246" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H246" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A247" s="32">
+        <v>1</v>
+      </c>
+      <c r="B247" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="C247" s="33">
+        <v>0.6</v>
+      </c>
+      <c r="D247" s="33">
+        <v>0.98889100346175773</v>
+      </c>
+      <c r="E247" s="33">
+        <f>C247*D247</f>
+        <v>0.59333460207705457</v>
+      </c>
+      <c r="F247" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G247" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H247" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A248" s="32">
+        <v>1</v>
+      </c>
+      <c r="B248" s="32">
+        <v>5</v>
+      </c>
+      <c r="C248" s="33">
+        <v>0.65</v>
+      </c>
+      <c r="D248" s="33">
+        <v>0.99326205300091452</v>
+      </c>
+      <c r="E248" s="33">
+        <f t="shared" ref="E248:E256" si="8">C248*D248</f>
+        <v>0.64562033445059441</v>
+      </c>
+      <c r="F248" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G248" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H248" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A249" s="32">
+        <v>1</v>
+      </c>
+      <c r="B249" s="32">
+        <v>5.5</v>
+      </c>
+      <c r="C249" s="33">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="D249" s="33">
+        <v>0.99591322856153597</v>
+      </c>
+      <c r="E249" s="33">
+        <f t="shared" si="8"/>
+        <v>0.67224142927903685</v>
+      </c>
+      <c r="F249" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G249" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H249" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A250" s="32">
+        <v>1</v>
+      </c>
+      <c r="B250" s="32">
+        <v>6</v>
+      </c>
+      <c r="C250" s="33">
+        <v>0.7</v>
+      </c>
+      <c r="D250" s="33">
+        <v>0.99752124782333362</v>
+      </c>
+      <c r="E250" s="33">
+        <f t="shared" si="8"/>
+        <v>0.69826487347633348</v>
+      </c>
+      <c r="F250" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G250" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H250" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A251" s="32">
+        <v>1</v>
+      </c>
+      <c r="B251" s="32">
+        <v>6.5</v>
+      </c>
+      <c r="C251" s="33">
+        <v>0.71</v>
+      </c>
+      <c r="D251" s="33">
+        <v>0.99849656080702243</v>
+      </c>
+      <c r="E251" s="33">
+        <f t="shared" si="8"/>
+        <v>0.70893255817298584</v>
+      </c>
+      <c r="F251" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G251" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H251" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A252" s="32">
+        <v>1</v>
+      </c>
+      <c r="B252" s="32">
+        <v>7</v>
+      </c>
+      <c r="C252" s="33">
+        <v>0.72</v>
+      </c>
+      <c r="D252" s="33">
+        <v>0.99908811803444553</v>
+      </c>
+      <c r="E252" s="33">
+        <f t="shared" si="8"/>
+        <v>0.71934344498480074</v>
+      </c>
+      <c r="F252" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G252" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H252" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A253" s="32">
+        <v>1</v>
+      </c>
+      <c r="B253" s="32">
+        <v>7.5</v>
+      </c>
+      <c r="C253" s="33">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D253" s="33">
+        <v>0.99944691562985222</v>
+      </c>
+      <c r="E253" s="33">
+        <f t="shared" si="8"/>
+        <v>0.72459901383164282</v>
+      </c>
+      <c r="F253" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G253" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H253" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A254" s="32">
+        <v>1</v>
+      </c>
+      <c r="B254" s="32">
+        <v>8</v>
+      </c>
+      <c r="C254" s="33">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D254" s="33">
+        <v>0.99966453737209748</v>
+      </c>
+      <c r="E254" s="33">
+        <f t="shared" si="8"/>
+        <v>0.72475678959477063</v>
+      </c>
+      <c r="F254" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G254" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H254" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A255" s="32">
+        <v>1</v>
+      </c>
+      <c r="B255" s="32">
+        <v>10</v>
+      </c>
+      <c r="C255" s="33">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D255" s="33">
+        <v>0.99995460007023751</v>
+      </c>
+      <c r="E255" s="33">
+        <f>C255*D255</f>
+        <v>0.72496708505092222</v>
+      </c>
+      <c r="F255" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G255" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H255" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A256" s="36">
+        <v>1</v>
+      </c>
+      <c r="B256" s="36">
+        <v>16</v>
+      </c>
+      <c r="C256" s="45">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D256" s="45">
+        <v>0.99999988746482527</v>
+      </c>
+      <c r="E256" s="45">
+        <f>C256*D256</f>
+        <v>0.72499991841199829</v>
+      </c>
+      <c r="F256" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G256" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H256" s="82" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HS (generic) in entity template added
some small improvements to hazard stats and plots
</commit_message>
<xml_diff>
--- a/data/entities/entity_template.xlsx
+++ b/data/entities/entity_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
     <sheet name="_discounting_sheet" sheetId="6" r:id="rId6"/>
     <sheet name="names" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150001" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -450,6 +450,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="H257" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>0161006, added</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -807,7 +820,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="113">
   <si>
     <t>Category_ID</t>
   </si>
@@ -1206,6 +1219,15 @@
   </si>
   <si>
     <t>Flood default</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>Ekin</t>
+  </si>
+  <si>
+    <t>Hail default</t>
   </si>
 </sst>
 </file>
@@ -2665,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:H272"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I243" sqref="I243"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G257" sqref="G257:H257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.33203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -9113,7 +9135,7 @@
         <v>0.39346934028736658</v>
       </c>
       <c r="E239" s="33">
-        <f t="shared" ref="E239:E254" si="7">C239*D239</f>
+        <f t="shared" ref="E239:E246" si="7">C239*D239</f>
         <v>3.9346934028736662E-3</v>
       </c>
       <c r="F239" s="34" t="s">
@@ -9356,7 +9378,7 @@
         <v>0.99326205300091452</v>
       </c>
       <c r="E248" s="33">
-        <f t="shared" ref="E248:E256" si="8">C248*D248</f>
+        <f t="shared" ref="E248:E254" si="8">C248*D248</f>
         <v>0.64562033445059441</v>
       </c>
       <c r="F248" s="34" t="s">
@@ -9583,6 +9605,438 @@
       </c>
       <c r="H256" s="82" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A257" s="31">
+        <v>1</v>
+      </c>
+      <c r="B257" s="31">
+        <v>0</v>
+      </c>
+      <c r="C257" s="31">
+        <v>0</v>
+      </c>
+      <c r="D257" s="31">
+        <v>0</v>
+      </c>
+      <c r="E257" s="31">
+        <f>C257*D257</f>
+        <v>0</v>
+      </c>
+      <c r="F257" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G257" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H257" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A258" s="31">
+        <v>1</v>
+      </c>
+      <c r="B258" s="31">
+        <v>200</v>
+      </c>
+      <c r="C258" s="31">
+        <v>0</v>
+      </c>
+      <c r="D258" s="31">
+        <v>0</v>
+      </c>
+      <c r="E258" s="31">
+        <f t="shared" ref="E258:E272" si="9">C258*D258</f>
+        <v>0</v>
+      </c>
+      <c r="F258" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G258" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H258" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A259" s="31">
+        <v>1</v>
+      </c>
+      <c r="B259" s="31">
+        <v>400</v>
+      </c>
+      <c r="C259" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="D259" s="31">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E259" s="31">
+        <f t="shared" si="9"/>
+        <v>1.0000000000000001E-7</v>
+      </c>
+      <c r="F259" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G259" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H259" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A260" s="31">
+        <v>1</v>
+      </c>
+      <c r="B260" s="31">
+        <v>600</v>
+      </c>
+      <c r="C260" s="31">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D260" s="31">
+        <v>1E-4</v>
+      </c>
+      <c r="E260" s="31">
+        <f t="shared" si="9"/>
+        <v>1.2000000000000002E-6</v>
+      </c>
+      <c r="F260" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G260" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H260" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A261" s="31">
+        <v>1</v>
+      </c>
+      <c r="B261" s="31">
+        <v>800</v>
+      </c>
+      <c r="C261" s="31">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D261" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="E261" s="31">
+        <f t="shared" si="9"/>
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="F261" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G261" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H261" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A262" s="31">
+        <v>1</v>
+      </c>
+      <c r="B262" s="31">
+        <v>1000</v>
+      </c>
+      <c r="C262" s="31">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D262" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="E262" s="31">
+        <f t="shared" si="9"/>
+        <v>1.4000000000000001E-4</v>
+      </c>
+      <c r="F262" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G262" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H262" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A263" s="31">
+        <v>1</v>
+      </c>
+      <c r="B263" s="31">
+        <v>1200</v>
+      </c>
+      <c r="C263" s="31">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D263" s="31">
+        <v>0.04</v>
+      </c>
+      <c r="E263" s="31">
+        <f t="shared" si="9"/>
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="F263" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G263" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H263" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A264" s="31">
+        <v>1</v>
+      </c>
+      <c r="B264" s="31">
+        <v>1400</v>
+      </c>
+      <c r="C264" s="31">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D264" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E264" s="31">
+        <f t="shared" si="9"/>
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="F264" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G264" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H264" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A265" s="31">
+        <v>1</v>
+      </c>
+      <c r="B265" s="31">
+        <v>1600</v>
+      </c>
+      <c r="C265" s="31">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D265" s="31">
+        <v>0.16</v>
+      </c>
+      <c r="E265" s="31">
+        <f t="shared" si="9"/>
+        <v>4.64E-3</v>
+      </c>
+      <c r="F265" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G265" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H265" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A266" s="31">
+        <v>1</v>
+      </c>
+      <c r="B266" s="31">
+        <v>1800</v>
+      </c>
+      <c r="C266" s="31">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D266" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="E266" s="31">
+        <f t="shared" si="9"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="F266" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G266" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H266" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A267" s="31">
+        <v>1</v>
+      </c>
+      <c r="B267" s="31">
+        <v>2000</v>
+      </c>
+      <c r="C267" s="31">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D267" s="31">
+        <v>0.27</v>
+      </c>
+      <c r="E267" s="31">
+        <f t="shared" si="9"/>
+        <v>1.2960000000000001E-2</v>
+      </c>
+      <c r="F267" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G267" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H267" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A268" s="31">
+        <v>1</v>
+      </c>
+      <c r="B268" s="31">
+        <v>2200</v>
+      </c>
+      <c r="C268" s="31">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D268" s="31">
+        <v>0.37</v>
+      </c>
+      <c r="E268" s="31">
+        <f t="shared" si="9"/>
+        <v>2.1829999999999999E-2</v>
+      </c>
+      <c r="F268" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G268" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H268" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A269" s="31">
+        <v>1</v>
+      </c>
+      <c r="B269" s="31">
+        <v>2400</v>
+      </c>
+      <c r="C269" s="31">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D269" s="31">
+        <v>0.49</v>
+      </c>
+      <c r="E269" s="31">
+        <f t="shared" si="9"/>
+        <v>3.4789999999999995E-2</v>
+      </c>
+      <c r="F269" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G269" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H269" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A270" s="31">
+        <v>1</v>
+      </c>
+      <c r="B270" s="31">
+        <v>2600</v>
+      </c>
+      <c r="C270" s="31">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="D270" s="31">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E270" s="31">
+        <f t="shared" si="9"/>
+        <v>5.1869999999999993E-2</v>
+      </c>
+      <c r="F270" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G270" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H270" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A271" s="31">
+        <v>1</v>
+      </c>
+      <c r="B271" s="31">
+        <v>2800</v>
+      </c>
+      <c r="C271" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D271" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="E271" s="31">
+        <f t="shared" si="9"/>
+        <v>0.06</v>
+      </c>
+      <c r="F271" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G271" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H271" s="82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A272" s="31">
+        <v>1</v>
+      </c>
+      <c r="B272" s="31">
+        <v>4000</v>
+      </c>
+      <c r="C272" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="D272" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="E272" s="31">
+        <f t="shared" si="9"/>
+        <v>0.06</v>
+      </c>
+      <c r="F272" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G272" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="H272" s="82" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BF (bushfire) default damage function added to template
and two minor edits
</commit_message>
<xml_diff>
--- a/data/entities/entity_template.xlsx
+++ b/data/entities/entity_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -463,6 +463,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="F273" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">added 20170623
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -820,7 +834,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="116">
   <si>
     <t>Category_ID</t>
   </si>
@@ -1229,17 +1243,27 @@
   <si>
     <t>Hail default</t>
   </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>brightness</t>
+  </si>
+  <si>
+    <t>bushfire default</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1468,7 +1492,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1558,6 +1582,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2687,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H272"/>
+  <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="90" workbookViewId="0">
-      <selection activeCell="G257" sqref="G257:H257"/>
+    <sheetView tabSelected="1" topLeftCell="A255" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A273" sqref="A273:H281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.33203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -10037,6 +10063,249 @@
       </c>
       <c r="H272" s="82" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A273" s="89">
+        <v>1</v>
+      </c>
+      <c r="B273" s="89">
+        <v>0</v>
+      </c>
+      <c r="C273" s="90">
+        <v>0</v>
+      </c>
+      <c r="D273" s="90">
+        <v>0</v>
+      </c>
+      <c r="E273" s="90">
+        <f>C273*D273</f>
+        <v>0</v>
+      </c>
+      <c r="F273" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G273" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H273" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A274" s="89">
+        <v>1</v>
+      </c>
+      <c r="B274" s="89">
+        <v>30</v>
+      </c>
+      <c r="C274" s="90">
+        <v>1E-4</v>
+      </c>
+      <c r="D274" s="90">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="E274" s="90">
+        <f t="shared" ref="E274:E281" si="10">C274*D274</f>
+        <v>2.5000000000000004E-7</v>
+      </c>
+      <c r="F274" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G274" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H274" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A275" s="89">
+        <v>1</v>
+      </c>
+      <c r="B275" s="89">
+        <v>50</v>
+      </c>
+      <c r="C275" s="90">
+        <v>1E-3</v>
+      </c>
+      <c r="D275" s="90">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E275" s="90">
+        <f t="shared" si="10"/>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="F275" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G275" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H275" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A276" s="89">
+        <v>1</v>
+      </c>
+      <c r="B276" s="89">
+        <v>100</v>
+      </c>
+      <c r="C276" s="90">
+        <v>0.01</v>
+      </c>
+      <c r="D276" s="90">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E276" s="90">
+        <f t="shared" si="10"/>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="F276" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G276" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H276" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A277" s="89">
+        <v>1</v>
+      </c>
+      <c r="B277" s="89">
+        <v>400</v>
+      </c>
+      <c r="C277" s="90">
+        <v>0.1</v>
+      </c>
+      <c r="D277" s="90">
+        <v>0.06</v>
+      </c>
+      <c r="E277" s="90">
+        <f t="shared" si="10"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F277" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G277" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H277" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A278" s="89">
+        <v>1</v>
+      </c>
+      <c r="B278" s="89">
+        <v>600</v>
+      </c>
+      <c r="C278" s="90">
+        <v>0.25</v>
+      </c>
+      <c r="D278" s="90">
+        <v>0.125</v>
+      </c>
+      <c r="E278" s="90">
+        <f t="shared" si="10"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="F278" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G278" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H278" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A279" s="89">
+        <v>1</v>
+      </c>
+      <c r="B279" s="89">
+        <v>800</v>
+      </c>
+      <c r="C279" s="90">
+        <v>0.45</v>
+      </c>
+      <c r="D279" s="90">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E279" s="90">
+        <f t="shared" si="10"/>
+        <v>7.8750000000000001E-2</v>
+      </c>
+      <c r="F279" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G279" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H279" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A280" s="89">
+        <v>1</v>
+      </c>
+      <c r="B280" s="89">
+        <v>1200</v>
+      </c>
+      <c r="C280" s="90">
+        <v>0.85</v>
+      </c>
+      <c r="D280" s="90">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E280" s="90">
+        <f t="shared" si="10"/>
+        <v>0.19125</v>
+      </c>
+      <c r="F280" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G280" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H280" s="89" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" ht="13" x14ac:dyDescent="0.15">
+      <c r="A281" s="89">
+        <v>1</v>
+      </c>
+      <c r="B281" s="89">
+        <v>1700</v>
+      </c>
+      <c r="C281" s="90">
+        <v>1</v>
+      </c>
+      <c r="D281" s="90">
+        <v>0.25</v>
+      </c>
+      <c r="E281" s="90">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+      <c r="F281" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="G281" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="H281" s="89" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
measuresID and DamageFunID added to names
</commit_message>
<xml_diff>
--- a/data/entities/entity_template.xlsx
+++ b/data/entities/entity_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="766" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="766"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
     <author>A satisfied Microsoft Office user</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -499,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -511,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -523,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -553,7 +553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -579,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -593,7 +593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -607,7 +607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -621,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -635,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -653,7 +653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -666,7 +666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -679,7 +679,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -692,7 +692,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -705,7 +705,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -718,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -773,6 +773,7 @@
   <authors>
     <author>A satisfied Microsoft Office user</author>
     <author>Microsoft Office User</author>
+    <author>David N. Bresch</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -829,12 +830,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="A5" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">to store further information for each damage function, like soure
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">to store further information for each damage function, like soure
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">to store further information for each measure like soure, range of applicability etc.
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="126">
   <si>
     <t>Category_ID</t>
   </si>
@@ -1252,6 +1295,36 @@
   <si>
     <t>bushfire default</t>
   </si>
+  <si>
+    <t>measureID</t>
+  </si>
+  <si>
+    <t>all default functions, based on expert judgement</t>
+  </si>
+  <si>
+    <t>demo damage function to reflect change in tropical cyclone (TC) buidling code, source expert judgement</t>
+  </si>
+  <si>
+    <t>beach nourishment, demo</t>
+  </si>
+  <si>
+    <t>vegetation management, demo</t>
+  </si>
+  <si>
+    <t>sandbags, demo</t>
+  </si>
+  <si>
+    <t>seawall, demo</t>
+  </si>
+  <si>
+    <t>elevate existing buildings, demo</t>
+  </si>
+  <si>
+    <t>enforce building code, demo, see DamageFunID 3</t>
+  </si>
+  <si>
+    <t>risk transfer, demo</t>
+  </si>
 </sst>
 </file>
 
@@ -1265,7 +1338,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1371,6 +1444,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="SwissReSans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1481,7 +1568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1491,6 +1578,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1585,10 +1676,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Comma 3" xfId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="5"/>
@@ -1939,9 +2034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2715,9 +2808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A273" sqref="A273:H281"/>
-    </sheetView>
+    <sheetView topLeftCell="A219" zoomScale="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.33203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10317,461 +10408,486 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="59" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="59" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="59" customWidth="1"/>
-    <col min="4" max="4" width="21" style="59" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="59" customWidth="1"/>
-    <col min="6" max="6" width="24" style="59" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="62" customWidth="1"/>
-    <col min="8" max="9" width="12.1640625" style="59" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" style="59" customWidth="1"/>
-    <col min="11" max="11" width="12" style="59" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" style="59" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="59" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" style="59" customWidth="1"/>
-    <col min="15" max="15" width="21" style="59" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="59" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" style="59" customWidth="1"/>
-    <col min="18" max="16384" width="11.5" style="59"/>
+    <col min="1" max="1" width="9.6640625" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="59" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="59" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="59" customWidth="1"/>
+    <col min="5" max="5" width="21" style="59" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="59" customWidth="1"/>
+    <col min="7" max="7" width="24" style="59" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="62" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" style="59" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" style="59" customWidth="1"/>
+    <col min="12" max="12" width="12" style="59" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" style="59" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" style="59" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="59" customWidth="1"/>
+    <col min="16" max="16" width="21" style="59" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" style="59" customWidth="1"/>
+    <col min="18" max="18" width="7.83203125" style="59" customWidth="1"/>
+    <col min="19" max="16384" width="11.5" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="58" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:18" s="58" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="C1" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="D1" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="E1" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="F1" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="G1" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="H1" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="I1" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="J1" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="K1" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="L1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="M1" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="83" t="s">
+      <c r="N1" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="83" t="s">
+      <c r="O1" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="70" t="s">
+      <c r="P1" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="Q1" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="R1" s="71" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A2" s="59" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A2" s="59">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="C2" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="74">
+      <c r="D2" s="74">
         <f>_measures_details!B15</f>
         <v>40572510.205771826</v>
       </c>
-      <c r="D2" s="84">
-        <v>1</v>
-      </c>
-      <c r="E2" s="75">
+      <c r="E2" s="84">
+        <v>1</v>
+      </c>
+      <c r="F2" s="75">
         <v>-1</v>
       </c>
-      <c r="F2" s="59">
-        <v>0</v>
-      </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="59">
+        <v>0</v>
+      </c>
+      <c r="H2" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="59">
-        <v>1</v>
-      </c>
       <c r="I2" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="59">
-        <v>0</v>
-      </c>
-      <c r="L2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="59">
+        <v>0</v>
+      </c>
+      <c r="M2" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="86" t="s">
+      <c r="N2" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="86">
-        <v>0</v>
-      </c>
-      <c r="O2" s="59">
+      <c r="O2" s="86">
         <v>0</v>
       </c>
       <c r="P2" s="59">
         <v>0</v>
       </c>
-      <c r="Q2" s="59" t="s">
+      <c r="Q2" s="59">
+        <v>0</v>
+      </c>
+      <c r="R2" s="59" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A3" s="59" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="59">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="C3" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="63">
+      <c r="D3" s="63">
         <f>_measures_details!B26</f>
         <v>63968125.006875344</v>
       </c>
-      <c r="D3" s="84">
-        <v>1</v>
-      </c>
-      <c r="E3" s="59">
+      <c r="E3" s="84">
+        <v>1</v>
+      </c>
+      <c r="F3" s="59">
         <v>-1</v>
       </c>
-      <c r="F3" s="59">
-        <v>0</v>
-      </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="59">
+        <v>0</v>
+      </c>
+      <c r="H3" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="59">
-        <v>1</v>
-      </c>
       <c r="I3" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="59">
+        <v>0</v>
+      </c>
+      <c r="K3" s="59">
         <v>0.8</v>
       </c>
-      <c r="K3" s="59">
-        <v>0</v>
-      </c>
-      <c r="L3" s="59" t="s">
+      <c r="L3" s="59">
+        <v>0</v>
+      </c>
+      <c r="M3" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="86" t="s">
+      <c r="N3" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="86">
-        <v>0</v>
-      </c>
-      <c r="O3" s="59">
+      <c r="O3" s="86">
         <v>0</v>
       </c>
       <c r="P3" s="59">
         <v>0</v>
       </c>
-      <c r="Q3" s="59" t="s">
+      <c r="Q3" s="59">
+        <v>0</v>
+      </c>
+      <c r="R3" s="59" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4" s="59">
+        <v>3</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="C4" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="63">
+      <c r="D4" s="63">
         <f>_measures_details!B34</f>
         <v>22388843.752406374</v>
       </c>
-      <c r="D4" s="84">
-        <v>1</v>
-      </c>
-      <c r="E4" s="59">
-        <v>0</v>
+      <c r="E4" s="84">
+        <v>1</v>
       </c>
       <c r="F4" s="59">
         <v>0</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="59">
+        <v>0</v>
+      </c>
+      <c r="H4" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="59">
+      <c r="I4" s="59">
         <v>0.9</v>
       </c>
-      <c r="I4" s="59">
-        <v>0</v>
-      </c>
       <c r="J4" s="59">
+        <v>0</v>
+      </c>
+      <c r="K4" s="59">
         <v>0.9</v>
       </c>
-      <c r="K4" s="59">
-        <v>0</v>
-      </c>
-      <c r="L4" s="59" t="s">
+      <c r="L4" s="59">
+        <v>0</v>
+      </c>
+      <c r="M4" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="86" t="s">
+      <c r="N4" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="86">
-        <v>0</v>
-      </c>
-      <c r="O4" s="59">
+      <c r="O4" s="86">
         <v>0</v>
       </c>
       <c r="P4" s="59">
         <v>0</v>
       </c>
-      <c r="Q4" s="59" t="s">
+      <c r="Q4" s="59">
+        <v>0</v>
+      </c>
+      <c r="R4" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A5" s="59" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5" s="59">
+        <v>4</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="C5" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="63">
+      <c r="D5" s="63">
         <f>_measures_details!B43</f>
         <v>731904375.02062607</v>
       </c>
-      <c r="D5" s="84">
-        <v>1</v>
-      </c>
-      <c r="E5" s="59">
-        <v>0</v>
+      <c r="E5" s="84">
+        <v>1</v>
       </c>
       <c r="F5" s="59">
+        <v>0</v>
+      </c>
+      <c r="G5" s="59">
         <f>1/15</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="H5" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="59">
-        <v>1</v>
-      </c>
       <c r="I5" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="59">
-        <v>0</v>
-      </c>
-      <c r="L5" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="59">
+        <v>0</v>
+      </c>
+      <c r="M5" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="86" t="s">
+      <c r="N5" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="86">
-        <v>0</v>
-      </c>
-      <c r="O5" s="59">
+      <c r="O5" s="86">
         <v>0</v>
       </c>
       <c r="P5" s="59">
         <v>0</v>
       </c>
-      <c r="Q5" s="59" t="s">
+      <c r="Q5" s="59">
+        <v>0</v>
+      </c>
+      <c r="R5" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A6" s="59" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6" s="59">
+        <v>5</v>
+      </c>
+      <c r="B6" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="C6" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="63">
+      <c r="D6" s="63">
         <f>_measures_details!B22</f>
         <v>3911963265.4766488</v>
       </c>
-      <c r="D6" s="84">
-        <v>1</v>
-      </c>
-      <c r="E6" s="59">
+      <c r="E6" s="84">
+        <v>1</v>
+      </c>
+      <c r="F6" s="59">
         <v>-2</v>
       </c>
-      <c r="F6" s="59">
-        <v>0</v>
-      </c>
-      <c r="G6" s="62" t="s">
+      <c r="G6" s="59">
+        <v>0</v>
+      </c>
+      <c r="H6" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="59">
+      <c r="I6" s="59">
         <v>0.9</v>
       </c>
-      <c r="I6" s="59">
+      <c r="J6" s="59">
         <v>-0.1</v>
       </c>
-      <c r="J6" s="59">
+      <c r="K6" s="59">
         <v>0.9</v>
       </c>
-      <c r="K6" s="59">
-        <v>0</v>
-      </c>
-      <c r="L6" s="59" t="s">
+      <c r="L6" s="59">
+        <v>0</v>
+      </c>
+      <c r="M6" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="86" t="s">
+      <c r="N6" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N6" s="86">
-        <v>0</v>
-      </c>
-      <c r="O6" s="59">
+      <c r="O6" s="86">
         <v>0</v>
       </c>
       <c r="P6" s="59">
         <v>0</v>
       </c>
-      <c r="Q6" s="59" t="s">
+      <c r="Q6" s="59">
+        <v>0</v>
+      </c>
+      <c r="R6" s="59" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A7" s="59" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="59">
+        <v>6</v>
+      </c>
+      <c r="B7" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="C7" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="63">
+      <c r="D7" s="63">
         <v>10000000</v>
       </c>
-      <c r="D7" s="84">
-        <v>1</v>
-      </c>
-      <c r="E7" s="59">
-        <v>0</v>
+      <c r="E7" s="84">
+        <v>1</v>
       </c>
       <c r="F7" s="59">
         <v>0</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="59">
+        <v>0</v>
+      </c>
+      <c r="H7" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="59">
-        <v>1</v>
-      </c>
       <c r="I7" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="59">
-        <v>0</v>
-      </c>
-      <c r="L7" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="59">
+        <v>0</v>
+      </c>
+      <c r="M7" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="86" t="s">
+      <c r="N7" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="86">
-        <v>0</v>
-      </c>
-      <c r="O7" s="59">
+      <c r="O7" s="86">
         <v>0</v>
       </c>
       <c r="P7" s="59">
         <v>0</v>
       </c>
-      <c r="Q7" s="59" t="s">
+      <c r="Q7" s="59">
+        <v>0</v>
+      </c>
+      <c r="R7" s="59" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A8" s="59" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8" s="59">
+        <v>7</v>
+      </c>
+      <c r="B8" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="C8" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="61">
-        <f>1000000+2%*P8</f>
+      <c r="D8" s="61">
+        <f>1000000+2%*Q8</f>
         <v>21000000</v>
       </c>
-      <c r="D8" s="84">
-        <v>1</v>
-      </c>
-      <c r="E8" s="59">
-        <v>0</v>
+      <c r="E8" s="84">
+        <v>1</v>
       </c>
       <c r="F8" s="59">
         <v>0</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="59">
+        <v>0</v>
+      </c>
+      <c r="H8" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="59">
-        <v>1</v>
-      </c>
       <c r="I8" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="59">
-        <v>0</v>
-      </c>
-      <c r="L8" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="59">
+        <v>0</v>
+      </c>
+      <c r="M8" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="86" t="s">
+      <c r="N8" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="86">
-        <v>0</v>
-      </c>
-      <c r="O8" s="61">
+      <c r="O8" s="86">
+        <v>0</v>
+      </c>
+      <c r="P8" s="61">
         <v>500000000</v>
       </c>
-      <c r="P8" s="61">
+      <c r="Q8" s="61">
         <v>1000000000</v>
       </c>
-      <c r="Q8" s="59" t="s">
+      <c r="R8" s="59" t="s">
         <v>17</v>
       </c>
     </row>
@@ -13169,17 +13285,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.83203125" bestFit="1" customWidth="1"/>
     <col min="257" max="261" width="10.83203125" customWidth="1"/>
     <col min="263" max="266" width="10.83203125" customWidth="1"/>
     <col min="269" max="269" width="10.83203125" customWidth="1"/>
@@ -15484,6 +15600,105 @@
         <v>2017</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="88">
+        <v>1</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="88">
+        <v>3</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="88">
+        <v>1</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="88">
+        <v>2</v>
+      </c>
+      <c r="C8" s="88" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="88">
+        <v>3</v>
+      </c>
+      <c r="C9" s="88" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="88">
+        <v>4</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="88">
+        <v>5</v>
+      </c>
+      <c r="C11" s="88" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="88">
+        <v>6</v>
+      </c>
+      <c r="C12" s="88" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="88">
+        <v>7</v>
+      </c>
+      <c r="C13" s="88" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>